<commit_message>
Updating genki study guide.
</commit_message>
<xml_diff>
--- a/linguistics/genki-study-resources/resources/tools/wordlist_E-J/lessons-3rd/lesson-14.xlsx
+++ b/linguistics/genki-study-resources/resources/tools/wordlist_E-J/lessons-3rd/lesson-14.xlsx
@@ -700,7 +700,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>résumé</t>
+          <t>resume; résumé</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -976,7 +976,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>I am no sure...</t>
+          <t>I am not sure...</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">

</xml_diff>